<commit_message>
Add some PS4 Data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Owner\Documents\GitHub\Y3-LLGP-RayTracer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s011120k\Documents\GitHub\Y3-LLGP-RayTracer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F6260B-3E6B-4430-837A-2372C079C80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095CE37D-C473-4B99-A408-484871E93BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Before</t>
   </si>
@@ -109,6 +109,12 @@
   <si>
     <t>Scene Optimised for Octree</t>
   </si>
+  <si>
+    <t>Time (in ms)</t>
+  </si>
+  <si>
+    <t>Subdivision Count</t>
+  </si>
 </sst>
 </file>
 
@@ -157,7 +163,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -175,7 +181,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -744,7 +750,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1160,7 +1166,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1932,7 +1938,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2606,7 +2612,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2981,6 +2987,531 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="382060079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PS4 Subdivision</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Count</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(scene</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>2.json, 3 worker threads)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (in ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$88:$B$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$88:$C$93</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1470</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1158</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1141</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6272-4084-9578-3A0D15ED0858}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="544949344"/>
+        <c:axId val="544960576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="544949344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Subdivision Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544960576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="544960576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Time</a:t>
+                </a:r>
+                <a:br>
+                  <a:rPr lang="en-GB"/>
+                </a:br>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>(of 10, in ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544949344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3236,6 +3767,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5262,6 +5833,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5946,6 +7020,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6A9AEB2-CCF6-FFF8-D4C0-ABAFDD169897}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6246,10 +7356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:D76"/>
+  <dimension ref="A5:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="P97" sqref="P97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6570,6 +7680,62 @@
         <v>511</v>
       </c>
     </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>5</v>
+      </c>
+      <c r="C93">
+        <v>1141</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B28:C34">
     <sortCondition descending="1" ref="B27:B34"/>

</xml_diff>